<commit_message>
Add more results for final models
</commit_message>
<xml_diff>
--- a/results/tables.xlsx
+++ b/results/tables.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\maestria-itam\segundo-semestre\modelos-lineales\examenes\2-covid\Spatial-Modeling\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E04A042-14CE-4966-A9B3-708B0B194039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA07354-EE15-44C2-822A-172E24F40E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E48CE3FD-34F7-49BE-A0E1-BA2FEEE3ADFB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{E48CE3FD-34F7-49BE-A0E1-BA2FEEE3ADFB}"/>
   </bookViews>
   <sheets>
     <sheet name="dics" sheetId="1" r:id="rId1"/>
     <sheet name="log_log_dics" sheetId="2" r:id="rId2"/>
+    <sheet name="car_proper_rho_90" sheetId="3" r:id="rId3"/>
+    <sheet name="car_proper_log_log_rho_90" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>car_proper_rho_90</t>
   </si>
@@ -81,13 +83,29 @@
   </si>
   <si>
     <t xml:space="preserve">    log( Y+1 ), log( E+1 )</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>beta_1</t>
+  </si>
+  <si>
+    <t>beta_2</t>
+  </si>
+  <si>
+    <t>Probability of 
+non-significance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +141,12 @@
       <name val="Avenir Next LT Pro"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Avenir Next LT Pro"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -144,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -152,10 +176,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -475,7 +511,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:A1048576"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,12 +523,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -504,7 +540,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -516,7 +552,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -528,7 +564,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -540,7 +576,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -552,7 +588,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -564,7 +600,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -576,7 +612,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -588,7 +624,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -600,7 +636,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -612,7 +648,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -636,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7557F128-E984-4F26-A9D7-FDAAF6C70505}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,12 +685,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -666,7 +702,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -677,7 +713,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -688,7 +724,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -699,7 +735,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -710,7 +746,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -721,7 +757,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -732,7 +768,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -743,19 +779,19 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="3"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="A11" s="3"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+      <c r="A12" s="3"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -767,4 +803,228 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08078B92-6EA8-47C4-83AA-08E18DCF3465}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D1" s="5">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.49236750000000001</v>
+      </c>
+      <c r="C2" s="8">
+        <v>-1.379</v>
+      </c>
+      <c r="D2" s="6">
+        <v>2.5369999999999999</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.25144443999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="8">
+        <v>-0.2389279</v>
+      </c>
+      <c r="C3" s="8">
+        <v>-0.56621250000000001</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.127</v>
+      </c>
+      <c r="E3" s="6">
+        <v>8.6666670000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE11CC4A-9D04-477A-BA0E-C8301D70C8F9}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D1" s="5">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="8">
+        <v>-0.2246958</v>
+      </c>
+      <c r="C2" s="8">
+        <v>-1.208</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.6764</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.29948150000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="8">
+        <v>-0.13376540000000001</v>
+      </c>
+      <c r="C3" s="8">
+        <v>-0.33879999999999999</v>
+      </c>
+      <c r="D3" s="6">
+        <v>8.2764249999999998E-2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.1009259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>